<commit_message>
add new monthly report type to unggah berkas
</commit_message>
<xml_diff>
--- a/static/Laporan Transaksi Bulanan Anggota Bursa.xlsx
+++ b/static/Laporan Transaksi Bulanan Anggota Bursa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irvan saharudin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TSG\AQI\bei-idx-portal-api-general-services\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804B1035-4598-4035-A097-A852D6E31D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15792C95-81F9-44E7-8D52-4DDE7C213B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5C5683F1-003B-4B0A-ABF7-6872F9BDDB18}"/>
   </bookViews>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F330FC-BF3B-43B0-82C4-D618081E52FB}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>